<commit_message>
Chagnes with tomorrow api
</commit_message>
<xml_diff>
--- a/Data_storage/Historical_weather.xlsx
+++ b/Data_storage/Historical_weather.xlsx
@@ -1,69 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\ruiz17\meteo\Data_storage\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17720D5-5C41-4829-B802-B771F23320F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="2024" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2024" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2025" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2026" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2027" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Mes</t>
-  </si>
-  <si>
-    <t>Dia</t>
-  </si>
-  <si>
-    <t>Hora</t>
-  </si>
-  <si>
-    <t>temp</t>
-  </si>
-  <si>
-    <t>hum</t>
-  </si>
-  <si>
-    <t>pres</t>
-  </si>
-  <si>
-    <t>wind_speed</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <b val="1"/>
       <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -97,24 +69,83 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -402,39 +433,521 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col width="10.140625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="5" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="11.85546875" bestFit="1" customWidth="1" min="7" max="7"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Mes</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Dia</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Hora</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>temp</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>hum</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>pres</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>wind_speed</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>15</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>17:00:02</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>7.87</v>
+      </c>
+      <c r="E2" t="n">
+        <v>73</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1038</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>15</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>17:30:02</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>7.77</v>
+      </c>
+      <c r="E3" t="n">
+        <v>72</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1038</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>15</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>18:00:02</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>7.21</v>
+      </c>
+      <c r="E4" t="n">
+        <v>75</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1038</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>15</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>18:30:03</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>6.44</v>
+      </c>
+      <c r="E5" t="n">
+        <v>78</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1039</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>15</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>19:00:02</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>4.77</v>
+      </c>
+      <c r="E6" t="n">
+        <v>81</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1039</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1.82</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>15</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>19:34:58</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>4.32</v>
+      </c>
+      <c r="E7" t="n">
+        <v>82</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1040</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>15</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>19:43:59</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>4.32</v>
+      </c>
+      <c r="E8" t="n">
+        <v>82</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1040</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>15</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>21:35:35</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>2.55</v>
+      </c>
+      <c r="E9" t="n">
+        <v>85</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1040</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0.24, 0.02, 0.16, 0.64, 3.94, 2.21, 1.48, 1.11, 0.89, 0.74, 0, 0, 0, 0.02, 0.01, 0.01, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>15</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>21:36:58</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>2.55</v>
+      </c>
+      <c r="E10" t="n">
+        <v>85</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1040</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0.24, 0.02, 0.16, 0.64, 3.94, 2.21, 1.48, 1.11, 0.89, 0.74, 0, 0, 0, 0.02, 0.01, 0.01, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>15</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>21:42:40</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>2.55</v>
+      </c>
+      <c r="E11" t="n">
+        <v>85</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1040</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>15</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>21:49:23</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="E12" t="n">
+        <v>85</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1040</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="H12" t="n">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>15</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>21:51:37</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>85</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1040</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>15</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>21:57:39</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>85</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1040</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>15</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>22:04:32</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>85</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1040</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.89</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Scripts to push and pull with rasp
</commit_message>
<xml_diff>
--- a/Data_storage/Historical_weather.xlsx
+++ b/Data_storage/Historical_weather.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
@@ -942,6 +942,486 @@
         <v>0.45</v>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>16</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>15:30:02</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>8.130000000000001</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>59</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1035</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>16</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>16:00:02</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>8.130000000000001</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>57</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1035</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>16</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>16:30:03</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>7.63</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>56</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1035</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>16</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>17:00:02</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>6.63</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>57</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1034</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>16</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>17:30:02</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>5.31</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>59</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1035</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>16</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>18:00:03</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>3.81</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>65</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1035</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>16</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>18:30:02</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>2.69</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" t="n">
+        <v>70</v>
+      </c>
+      <c r="G23" t="n">
+        <v>1035</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>16</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>19:00:02</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>1.88</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>73</v>
+      </c>
+      <c r="G24" t="n">
+        <v>1035</v>
+      </c>
+      <c r="H24" t="n">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>16</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>19:30:02</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>76</v>
+      </c>
+      <c r="G25" t="n">
+        <v>1036</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>16</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>20:00:02</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>-0.38</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>78</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1036</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>16</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>20:30:02</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>-0.6899999999999999</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>78</v>
+      </c>
+      <c r="G27" t="n">
+        <v>1036</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>16</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>21:00:02</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>-0.88</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>82</v>
+      </c>
+      <c r="G28" t="n">
+        <v>1036</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>16</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>21:30:02</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>-1.13</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" t="n">
+        <v>83</v>
+      </c>
+      <c r="G29" t="n">
+        <v>1036</v>
+      </c>
+      <c r="H29" t="n">
+        <v>1.15</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>16</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>22:00:02</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>-1.19</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>83</v>
+      </c>
+      <c r="G30" t="n">
+        <v>1036</v>
+      </c>
+      <c r="H30" t="n">
+        <v>1.15</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>16</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>22:42:25</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>-1.5</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>83</v>
+      </c>
+      <c r="G31" t="n">
+        <v>1036</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>16</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>23:00:06</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>-1.5</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>83</v>
+      </c>
+      <c r="G32" t="n">
+        <v>1036</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Implementacion de reintentos de peticion API
</commit_message>
<xml_diff>
--- a/Data_storage/Historical_weather.xlsx
+++ b/Data_storage/Historical_weather.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H73"/>
+  <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
@@ -2652,6 +2652,36 @@
         <v>1.34</v>
       </c>
     </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>17</v>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>19:52:08</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="E74" t="n">
+        <v>0</v>
+      </c>
+      <c r="F74" t="n">
+        <v>70</v>
+      </c>
+      <c r="G74" t="n">
+        <v>1031</v>
+      </c>
+      <c r="H74" t="n">
+        <v>2.24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Introduccion del datavisulizer y reconfiguracion de carpetas, si todo en el mismo commit
</commit_message>
<xml_diff>
--- a/Data_storage/Historical_weather.xlsx
+++ b/Data_storage/Historical_weather.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H74"/>
+  <dimension ref="A1:H79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
@@ -2633,23 +2633,23 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>19:40:59</t>
+          <t>20:00:04</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>1.38</v>
+        <v>1.13</v>
       </c>
       <c r="E73" t="n">
         <v>0</v>
       </c>
       <c r="F73" t="n">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G73" t="n">
         <v>1031</v>
       </c>
       <c r="H73" t="n">
-        <v>1.34</v>
+        <v>2.24</v>
       </c>
     </row>
     <row r="74">
@@ -2663,23 +2663,173 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>19:52:08</t>
+          <t>20:30:05</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>1.13</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E74" t="n">
         <v>0</v>
       </c>
       <c r="F74" t="n">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G74" t="n">
         <v>1031</v>
       </c>
       <c r="H74" t="n">
-        <v>2.24</v>
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>17</v>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>21:00:05</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0</v>
+      </c>
+      <c r="F75" t="n">
+        <v>76</v>
+      </c>
+      <c r="G75" t="n">
+        <v>1031</v>
+      </c>
+      <c r="H75" t="n">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>17</v>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>21:30:07</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0</v>
+      </c>
+      <c r="F76" t="n">
+        <v>77</v>
+      </c>
+      <c r="G76" t="n">
+        <v>1031</v>
+      </c>
+      <c r="H76" t="n">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>17</v>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>22:00:05</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0</v>
+      </c>
+      <c r="F77" t="n">
+        <v>78</v>
+      </c>
+      <c r="G77" t="n">
+        <v>1031</v>
+      </c>
+      <c r="H77" t="n">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>17</v>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>22:30:04</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0</v>
+      </c>
+      <c r="F78" t="n">
+        <v>80</v>
+      </c>
+      <c r="G78" t="n">
+        <v>1031</v>
+      </c>
+      <c r="H78" t="n">
+        <v>2.05</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>17</v>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>23:00:05</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0</v>
+      </c>
+      <c r="F79" t="n">
+        <v>81</v>
+      </c>
+      <c r="G79" t="n">
+        <v>1031</v>
+      </c>
+      <c r="H79" t="n">
+        <v>2.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>